<commit_message>
Added new scripts for genes
</commit_message>
<xml_diff>
--- a/dna-methylation/scripts/develop/betas/plot/scatter_comparison_rows.xlsx
+++ b/dna-methylation/scripts/develop/betas/plot/scatter_comparison_rows.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21727"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\dna-methylation\dna-methylation\scripts\develop\betas\plot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2F9B7F-01B8-4988-B229-CBD00AA5C8A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16689" yWindow="8863" windowWidth="16225" windowHeight="9051" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16689" yWindow="8863" windowWidth="16226" windowHeight="9051"/>
   </bookViews>
   <sheets>
     <sheet name="i" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>begins</t>
   </si>
@@ -34,49 +33,19 @@
     <t>aux</t>
   </si>
   <si>
-    <t>cg13382567</t>
-  </si>
-  <si>
-    <t>cg25887789</t>
-  </si>
-  <si>
-    <t>cg01302668</t>
-  </si>
-  <si>
-    <t>cg00134667</t>
-  </si>
-  <si>
-    <t>cg25364822</t>
-  </si>
-  <si>
-    <t>cg18557131</t>
-  </si>
-  <si>
-    <t>SRRM4</t>
-  </si>
-  <si>
-    <t>PDZRN4</t>
-  </si>
-  <si>
-    <t>FAM162B</t>
-  </si>
-  <si>
-    <t>CACNA1H</t>
-  </si>
-  <si>
-    <t>FNDC5</t>
-  </si>
-  <si>
-    <t>ZIC5</t>
-  </si>
-  <si>
     <t>auto</t>
+  </si>
+  <si>
+    <t>cg05072008</t>
+  </si>
+  <si>
+    <t>FIGNL1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -227,23 +196,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -279,23 +231,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -471,11 +406,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.53515625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -496,86 +431,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
       <c r="D2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>